<commit_message>
added hyphen to workbook names
</commit_message>
<xml_diff>
--- a/stockPortfolio.xlsx
+++ b/stockPortfolio.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\葉怡成\C_disk\Documents and Settings\icyeh\My Documents\project\UCI Data Set 捐贈\6 stock selection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/novoachampion/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1754186A-0452-CF42-A662-6EE1C144A686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23160" windowHeight="11260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="4th period" sheetId="8" r:id="rId1"/>
@@ -243,15 +244,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="186" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -264,7 +265,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="新細明體"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -437,16 +438,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -455,20 +456,14 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -479,12 +474,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -761,48 +762,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="9.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="9.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="27" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-    </row>
-    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+    </row>
+    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -861,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -920,7 +921,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -979,7 +980,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1038,7 +1039,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1097,7 +1098,7 @@
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1156,7 +1157,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1215,7 +1216,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1274,7 +1275,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1333,7 +1334,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1392,7 +1393,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1510,7 +1511,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1569,7 +1570,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1687,7 +1688,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -1746,7 +1747,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -1864,7 +1865,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -1923,7 +1924,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -1982,7 +1983,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -2041,7 +2042,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -2100,7 +2101,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -2159,7 +2160,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2218,7 +2219,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -2277,7 +2278,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -2336,7 +2337,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -2395,7 +2396,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -2513,7 +2514,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -2572,7 +2573,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -2631,7 +2632,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -2690,7 +2691,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -2749,7 +2750,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2808,7 +2809,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -2867,7 +2868,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -2926,7 +2927,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -2985,7 +2986,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -3044,7 +3045,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -3103,7 +3104,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -3162,7 +3163,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -3280,7 +3281,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -3339,7 +3340,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -3398,7 +3399,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -3457,7 +3458,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -3516,7 +3517,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -3575,7 +3576,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -3634,7 +3635,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -3693,7 +3694,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -3752,7 +3753,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -3811,7 +3812,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -3870,7 +3871,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -3929,7 +3930,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -3988,7 +3989,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -4047,7 +4048,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -4106,7 +4107,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -4165,7 +4166,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -4224,7 +4225,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -4283,7 +4284,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -4342,7 +4343,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -4401,7 +4402,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -4460,7 +4461,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -4519,7 +4520,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -4590,48 +4591,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3:S65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="9.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="9.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="27" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-    </row>
-    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+    </row>
+    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4690,7 +4691,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -4749,7 +4750,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -4808,7 +4809,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -4867,7 +4868,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -4926,7 +4927,7 @@
         <v>0.27500000000000008</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -4985,7 +4986,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -5044,7 +5045,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -5103,7 +5104,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -5162,7 +5163,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -5221,7 +5222,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -5280,7 +5281,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -5339,7 +5340,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -5398,7 +5399,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -5457,7 +5458,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -5516,7 +5517,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -5575,7 +5576,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -5634,7 +5635,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -5693,7 +5694,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -5752,7 +5753,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -5811,7 +5812,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -5870,7 +5871,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -5929,7 +5930,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -5988,7 +5989,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -6047,7 +6048,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -6106,7 +6107,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -6165,7 +6166,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -6224,7 +6225,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -6283,7 +6284,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -6342,7 +6343,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -6401,7 +6402,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -6460,7 +6461,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -6519,7 +6520,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -6578,7 +6579,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -6637,7 +6638,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -6696,7 +6697,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -6755,7 +6756,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -6814,7 +6815,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -6873,7 +6874,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -6932,7 +6933,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -6991,7 +6992,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -7050,7 +7051,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -7109,7 +7110,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -7168,7 +7169,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -7227,7 +7228,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -7286,7 +7287,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -7345,7 +7346,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -7404,7 +7405,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -7463,7 +7464,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -7522,7 +7523,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -7581,7 +7582,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -7640,7 +7641,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -7699,7 +7700,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -7758,7 +7759,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -7817,7 +7818,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -7876,7 +7877,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -7935,7 +7936,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -7994,7 +7995,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -8053,7 +8054,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -8112,7 +8113,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -8171,7 +8172,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -8230,7 +8231,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -8289,7 +8290,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -8348,7 +8349,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -8419,48 +8420,48 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3:S65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="9.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="9.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="27" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-    </row>
-    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+    </row>
+    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -8519,7 +8520,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -8578,7 +8579,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -8637,7 +8638,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -8696,7 +8697,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -8755,7 +8756,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -8814,7 +8815,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -8873,7 +8874,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -8932,7 +8933,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -8991,7 +8992,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -9050,7 +9051,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -9109,7 +9110,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -9168,7 +9169,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -9227,7 +9228,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -9286,7 +9287,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -9345,7 +9346,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -9404,7 +9405,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -9463,7 +9464,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -9522,7 +9523,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -9581,7 +9582,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -9640,7 +9641,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -9699,7 +9700,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -9758,7 +9759,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -9817,7 +9818,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -9876,7 +9877,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -9935,7 +9936,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -9994,7 +9995,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -10053,7 +10054,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -10112,7 +10113,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -10171,7 +10172,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -10230,7 +10231,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -10289,7 +10290,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -10348,7 +10349,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -10407,7 +10408,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -10466,7 +10467,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -10525,7 +10526,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -10584,7 +10585,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -10643,7 +10644,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -10702,7 +10703,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -10761,7 +10762,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -10820,7 +10821,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -10879,7 +10880,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -10938,7 +10939,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -10997,7 +10998,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -11056,7 +11057,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -11115,7 +11116,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -11174,7 +11175,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -11233,7 +11234,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -11292,7 +11293,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -11351,7 +11352,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -11410,7 +11411,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -11469,7 +11470,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -11528,7 +11529,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -11587,7 +11588,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -11646,7 +11647,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -11705,7 +11706,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -11764,7 +11765,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -11823,7 +11824,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -11882,7 +11883,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -11941,7 +11942,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -12000,7 +12001,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -12059,7 +12060,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -12118,7 +12119,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -12177,7 +12178,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -12248,49 +12249,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S68"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="9" width="9.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.375" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.125" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="10.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="10.1640625" style="11" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="21" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="22" t="s">
+    <row r="1" spans="1:19" s="21" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="23" t="s">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="24" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="24"/>
-      <c r="P1" s="24"/>
-      <c r="Q1" s="24"/>
-      <c r="R1" s="24"/>
-      <c r="S1" s="24"/>
-    </row>
-    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+    </row>
+    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -12349,7 +12350,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -12408,7 +12409,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -12467,7 +12468,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -12526,7 +12527,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -12585,7 +12586,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -12644,7 +12645,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -12703,7 +12704,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -12762,7 +12763,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -12821,7 +12822,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -12880,7 +12881,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -12939,7 +12940,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -12998,7 +12999,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -13057,7 +13058,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -13116,7 +13117,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -13175,7 +13176,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -13234,7 +13235,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -13293,7 +13294,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -13352,7 +13353,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -13411,7 +13412,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -13470,7 +13471,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -13529,7 +13530,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -13588,7 +13589,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -13647,7 +13648,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -13706,7 +13707,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -13765,7 +13766,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -13824,7 +13825,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -13883,7 +13884,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -13942,7 +13943,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -14001,7 +14002,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -14060,7 +14061,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -14119,7 +14120,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -14178,7 +14179,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -14237,7 +14238,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -14296,7 +14297,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -14355,7 +14356,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -14414,7 +14415,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -14473,7 +14474,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -14532,7 +14533,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -14591,7 +14592,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -14650,7 +14651,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -14709,7 +14710,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -14768,7 +14769,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -14827,7 +14828,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -14886,7 +14887,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -14945,7 +14946,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -15004,7 +15005,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -15063,7 +15064,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -15122,7 +15123,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -15181,7 +15182,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -15240,7 +15241,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -15299,7 +15300,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -15358,7 +15359,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -15417,7 +15418,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -15476,7 +15477,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -15535,7 +15536,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -15594,7 +15595,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -15653,7 +15654,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -15712,7 +15713,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -15771,7 +15772,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -15830,7 +15831,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -15889,7 +15890,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -15948,7 +15949,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -16007,7 +16008,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -16066,7 +16067,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
       <c r="N67" s="20"/>
       <c r="O67" s="20"/>
       <c r="P67" s="20"/>
@@ -16074,7 +16075,7 @@
       <c r="R67" s="20"/>
       <c r="S67" s="20"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
       <c r="N68" s="20"/>
       <c r="O68" s="20"/>
       <c r="P68" s="20"/>
@@ -16094,45 +16095,45 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3:S65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="26" t="s">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="27" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-    </row>
-    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+    </row>
+    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -16191,7 +16192,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -16250,7 +16251,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -16309,7 +16310,7 @@
         <v>0.76470588235294135</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -16368,7 +16369,7 @@
         <v>0.376470588235294</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -16427,7 +16428,7 @@
         <v>0.27058823529411757</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -16486,7 +16487,7 @@
         <v>0.44705882352941173</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -16545,7 +16546,7 @@
         <v>0.23529411764705888</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -16604,7 +16605,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -16663,7 +16664,7 @@
         <v>0.376470588235294</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -16722,7 +16723,7 @@
         <v>0.76470588235294135</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -16781,7 +16782,7 @@
         <v>0.376470588235294</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -16840,7 +16841,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -16899,7 +16900,7 @@
         <v>0.51764705882352935</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -16958,7 +16959,7 @@
         <v>0.55294117647058805</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -17017,7 +17018,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -17076,7 +17077,7 @@
         <v>0.51764705882352935</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -17135,7 +17136,7 @@
         <v>0.3411764705882353</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -17194,7 +17195,7 @@
         <v>0.3411764705882353</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -17253,7 +17254,7 @@
         <v>0.69411764705882351</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -17312,7 +17313,7 @@
         <v>0.48235294117647071</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -17371,7 +17372,7 @@
         <v>0.30588235294117644</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -17430,7 +17431,7 @@
         <v>0.3411764705882353</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -17489,7 +17490,7 @@
         <v>0.76470588235294135</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -17548,7 +17549,7 @@
         <v>0.55294117647058805</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -17607,7 +17608,7 @@
         <v>0.30588235294117644</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -17666,7 +17667,7 @@
         <v>0.65882352941176481</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -17725,7 +17726,7 @@
         <v>0.69411764705882351</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -17784,7 +17785,7 @@
         <v>0.58823529411764719</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -17843,7 +17844,7 @@
         <v>0.62352941176470589</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -17902,7 +17903,7 @@
         <v>0.44705882352941173</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -17961,7 +17962,7 @@
         <v>0.58823529411764719</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -18020,7 +18021,7 @@
         <v>0.62352941176470589</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -18079,7 +18080,7 @@
         <v>0.51764705882352935</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -18138,7 +18139,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -18197,7 +18198,7 @@
         <v>0.58823529411764719</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -18256,7 +18257,7 @@
         <v>0.48235294117647071</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -18315,7 +18316,7 @@
         <v>0.55294117647058805</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -18374,7 +18375,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -18433,7 +18434,7 @@
         <v>0.48235294117647071</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -18492,7 +18493,7 @@
         <v>0.69411764705882351</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -18551,7 +18552,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -18610,7 +18611,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -18669,7 +18670,7 @@
         <v>0.55294117647058805</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -18728,7 +18729,7 @@
         <v>0.76470588235294135</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -18787,7 +18788,7 @@
         <v>0.65882352941176481</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -18846,7 +18847,7 @@
         <v>0.44705882352941173</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -18905,7 +18906,7 @@
         <v>0.69411764705882351</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -18964,7 +18965,7 @@
         <v>0.58823529411764719</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -19023,7 +19024,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -19082,7 +19083,7 @@
         <v>0.376470588235294</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -19141,7 +19142,7 @@
         <v>0.65882352941176481</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -19200,7 +19201,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -19259,7 +19260,7 @@
         <v>0.62352941176470589</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -19318,7 +19319,7 @@
         <v>0.69411764705882351</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -19377,7 +19378,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -19436,7 +19437,7 @@
         <v>0.51764705882352935</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -19495,7 +19496,7 @@
         <v>0.44705882352941173</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -19554,7 +19555,7 @@
         <v>0.62352941176470589</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -19613,7 +19614,7 @@
         <v>0.55294117647058805</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -19672,7 +19673,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -19731,7 +19732,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -19790,7 +19791,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -19849,7 +19850,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -19920,19 +19921,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="20.625" customWidth="1"/>
+    <col min="1" max="4" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -19946,70 +19947,70 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="22" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="22" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="22" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="22" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="22" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="10" t="s">

</xml_diff>

<commit_message>
created modules to run dif parts of training and prep
</commit_message>
<xml_diff>
--- a/stockPortfolio.xlsx
+++ b/stockPortfolio.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/novoachampion/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\葉怡成\C_disk\Documents and Settings\icyeh\My Documents\project\UCI Data Set 捐贈\6 stock selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1754186A-0452-CF42-A662-6EE1C144A686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23160" windowHeight="11260" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="4th period" sheetId="8" r:id="rId1"/>
@@ -244,15 +243,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="186" formatCode="0.000"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -265,7 +264,7 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="新細明體"/>
       <family val="2"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -438,16 +437,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="186" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="186" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="186" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="186" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -456,14 +455,20 @@
     <xf numFmtId="10" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="186" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -474,18 +479,12 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="17" fontId="6" fillId="0" borderId="4" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="一般" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -762,48 +761,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="9.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.375" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="9.125" style="11" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="25" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-    </row>
-    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+    </row>
+    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -862,7 +861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -921,7 +920,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -980,7 +979,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -1039,7 +1038,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -1098,7 +1097,7 @@
         <v>0.26666666666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -1157,7 +1156,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1216,7 +1215,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1275,7 +1274,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1334,7 +1333,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1393,7 +1392,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1452,7 +1451,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1511,7 +1510,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1570,7 +1569,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1629,7 +1628,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1688,7 +1687,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -1747,7 +1746,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -1865,7 +1864,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -1924,7 +1923,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -1983,7 +1982,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -2042,7 +2041,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -2101,7 +2100,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -2160,7 +2159,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -2219,7 +2218,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -2278,7 +2277,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -2337,7 +2336,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -2396,7 +2395,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -2455,7 +2454,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -2514,7 +2513,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -2573,7 +2572,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -2691,7 +2690,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -2750,7 +2749,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -2809,7 +2808,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -2868,7 +2867,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -2927,7 +2926,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -2986,7 +2985,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -3045,7 +3044,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -3104,7 +3103,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -3163,7 +3162,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -3222,7 +3221,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -3281,7 +3280,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -3340,7 +3339,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -3399,7 +3398,7 @@
         <v>0.73333333333333339</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -3458,7 +3457,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -3517,7 +3516,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -3576,7 +3575,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -3635,7 +3634,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -3694,7 +3693,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -3753,7 +3752,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -3812,7 +3811,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -3871,7 +3870,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -3930,7 +3929,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -3989,7 +3988,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -4048,7 +4047,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -4107,7 +4106,7 @@
         <v>0.33333333333333337</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -4166,7 +4165,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -4225,7 +4224,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -4284,7 +4283,7 @@
         <v>0.53333333333333344</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -4343,7 +4342,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -4402,7 +4401,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -4461,7 +4460,7 @@
         <v>0.46666666666666667</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -4520,7 +4519,7 @@
         <v>0.66666666666666674</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -4591,48 +4590,48 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3:S65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="9.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.375" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="9.125" style="11" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="25" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-    </row>
-    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+    </row>
+    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -4691,7 +4690,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -4750,7 +4749,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -4809,7 +4808,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -4868,7 +4867,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -4927,7 +4926,7 @@
         <v>0.27500000000000008</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -4986,7 +4985,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -5045,7 +5044,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -5104,7 +5103,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -5163,7 +5162,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -5222,7 +5221,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -5281,7 +5280,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -5340,7 +5339,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -5399,7 +5398,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -5458,7 +5457,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -5517,7 +5516,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -5576,7 +5575,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -5635,7 +5634,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -5694,7 +5693,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -5753,7 +5752,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -5812,7 +5811,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -5871,7 +5870,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -5930,7 +5929,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -5989,7 +5988,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -6048,7 +6047,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -6107,7 +6106,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -6166,7 +6165,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -6225,7 +6224,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -6284,7 +6283,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -6343,7 +6342,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -6402,7 +6401,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -6461,7 +6460,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -6520,7 +6519,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -6579,7 +6578,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -6638,7 +6637,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -6697,7 +6696,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -6756,7 +6755,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -6815,7 +6814,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -6874,7 +6873,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -6933,7 +6932,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -6992,7 +6991,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -7051,7 +7050,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -7110,7 +7109,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -7169,7 +7168,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -7228,7 +7227,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -7287,7 +7286,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -7346,7 +7345,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -7405,7 +7404,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -7464,7 +7463,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -7523,7 +7522,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -7582,7 +7581,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -7641,7 +7640,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -7700,7 +7699,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -7759,7 +7758,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -7818,7 +7817,7 @@
         <v>0.65000000000000013</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -7877,7 +7876,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -7936,7 +7935,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -7995,7 +7994,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -8054,7 +8053,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -8113,7 +8112,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -8172,7 +8171,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -8231,7 +8230,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -8290,7 +8289,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -8349,7 +8348,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -8420,48 +8419,48 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3:S65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="19" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="9.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.375" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="19" width="9.125" style="11" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="25" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-    </row>
-    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+    </row>
+    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -8520,7 +8519,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -8579,7 +8578,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -8638,7 +8637,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -8697,7 +8696,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -8756,7 +8755,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -8815,7 +8814,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -8874,7 +8873,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -8933,7 +8932,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -8992,7 +8991,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -9051,7 +9050,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -9110,7 +9109,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -9169,7 +9168,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -9228,7 +9227,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -9287,7 +9286,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -9346,7 +9345,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -9405,7 +9404,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -9464,7 +9463,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -9523,7 +9522,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -9582,7 +9581,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -9641,7 +9640,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -9700,7 +9699,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -9759,7 +9758,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -9818,7 +9817,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -9877,7 +9876,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -9936,7 +9935,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -9995,7 +9994,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -10054,7 +10053,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -10113,7 +10112,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -10172,7 +10171,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -10231,7 +10230,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -10290,7 +10289,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -10349,7 +10348,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -10408,7 +10407,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -10467,7 +10466,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -10526,7 +10525,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -10585,7 +10584,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -10644,7 +10643,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -10703,7 +10702,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -10762,7 +10761,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -10821,7 +10820,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -10880,7 +10879,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -10939,7 +10938,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -10998,7 +10997,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -11057,7 +11056,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -11116,7 +11115,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -11175,7 +11174,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -11234,7 +11233,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -11293,7 +11292,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -11352,7 +11351,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -11411,7 +11410,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -11470,7 +11469,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -11529,7 +11528,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -11588,7 +11587,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -11647,7 +11646,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -11706,7 +11705,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -11765,7 +11764,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -11824,7 +11823,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -11883,7 +11882,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -11942,7 +11941,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -12001,7 +12000,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -12060,7 +12059,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -12119,7 +12118,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -12178,7 +12177,7 @@
         <v>0.39999999999999997</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -12249,49 +12248,49 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S68"/>
   <sheetViews>
     <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="9.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="19" width="10.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="9" width="9.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.375" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="9.125" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="19" width="10.125" style="11" bestFit="1" customWidth="1"/>
     <col min="20" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="21" customFormat="1" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="28" t="s">
+    <row r="1" spans="1:19" s="21" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="26" t="s">
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="27" t="s">
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-    </row>
-    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+    </row>
+    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -12350,7 +12349,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -12409,7 +12408,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -12468,7 +12467,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -12527,7 +12526,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -12586,7 +12585,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -12645,7 +12644,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -12704,7 +12703,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -12763,7 +12762,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -12822,7 +12821,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -12881,7 +12880,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -12940,7 +12939,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -12999,7 +12998,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -13058,7 +13057,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -13117,7 +13116,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -13176,7 +13175,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -13235,7 +13234,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -13294,7 +13293,7 @@
         <v>0.27500000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -13353,7 +13352,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -13412,7 +13411,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -13471,7 +13470,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -13530,7 +13529,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -13589,7 +13588,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -13648,7 +13647,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -13707,7 +13706,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -13766,7 +13765,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -13825,7 +13824,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -13884,7 +13883,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -13943,7 +13942,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -14002,7 +14001,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -14061,7 +14060,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -14120,7 +14119,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -14179,7 +14178,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -14238,7 +14237,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -14297,7 +14296,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -14356,7 +14355,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -14415,7 +14414,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -14474,7 +14473,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -14533,7 +14532,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -14592,7 +14591,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -14651,7 +14650,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -14710,7 +14709,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -14769,7 +14768,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -14828,7 +14827,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -14887,7 +14886,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -14946,7 +14945,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -15005,7 +15004,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -15064,7 +15063,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -15123,7 +15122,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -15182,7 +15181,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -15241,7 +15240,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -15300,7 +15299,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -15359,7 +15358,7 @@
         <v>0.72499999999999987</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -15418,7 +15417,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -15477,7 +15476,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -15536,7 +15535,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -15595,7 +15594,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -15654,7 +15653,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -15713,7 +15712,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -15772,7 +15771,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -15831,7 +15830,7 @@
         <v>0.57499999999999996</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -15890,7 +15889,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -15949,7 +15948,7 @@
         <v>0.42500000000000004</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -16008,7 +16007,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -16067,7 +16066,7 @@
         <v>0.64999999999999991</v>
       </c>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N67" s="20"/>
       <c r="O67" s="20"/>
       <c r="P67" s="20"/>
@@ -16075,7 +16074,7 @@
       <c r="R67" s="20"/>
       <c r="S67" s="20"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="N68" s="20"/>
       <c r="O68" s="20"/>
       <c r="P68" s="20"/>
@@ -16095,45 +16094,45 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S65"/>
   <sheetViews>
     <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="N3" sqref="N3:S65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="9" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="23" t="s">
+    <row r="1" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="24" t="s">
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="25" t="s">
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-    </row>
-    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="27"/>
+    </row>
+    <row r="2" spans="1:19" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -16192,7 +16191,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -16251,7 +16250,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -16310,7 +16309,7 @@
         <v>0.76470588235294135</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -16369,7 +16368,7 @@
         <v>0.376470588235294</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -16428,7 +16427,7 @@
         <v>0.27058823529411757</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -16487,7 +16486,7 @@
         <v>0.44705882352941173</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -16546,7 +16545,7 @@
         <v>0.23529411764705888</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -16605,7 +16604,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -16664,7 +16663,7 @@
         <v>0.376470588235294</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -16723,7 +16722,7 @@
         <v>0.76470588235294135</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -16782,7 +16781,7 @@
         <v>0.376470588235294</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -16841,7 +16840,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -16900,7 +16899,7 @@
         <v>0.51764705882352935</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -16959,7 +16958,7 @@
         <v>0.55294117647058805</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -17018,7 +17017,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -17077,7 +17076,7 @@
         <v>0.51764705882352935</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -17136,7 +17135,7 @@
         <v>0.3411764705882353</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -17195,7 +17194,7 @@
         <v>0.3411764705882353</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -17254,7 +17253,7 @@
         <v>0.69411764705882351</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -17313,7 +17312,7 @@
         <v>0.48235294117647071</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -17372,7 +17371,7 @@
         <v>0.30588235294117644</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -17431,7 +17430,7 @@
         <v>0.3411764705882353</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -17490,7 +17489,7 @@
         <v>0.76470588235294135</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -17549,7 +17548,7 @@
         <v>0.55294117647058805</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -17608,7 +17607,7 @@
         <v>0.30588235294117644</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -17667,7 +17666,7 @@
         <v>0.65882352941176481</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -17726,7 +17725,7 @@
         <v>0.69411764705882351</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -17785,7 +17784,7 @@
         <v>0.58823529411764719</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -17844,7 +17843,7 @@
         <v>0.62352941176470589</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -17903,7 +17902,7 @@
         <v>0.44705882352941173</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>30</v>
       </c>
@@ -17962,7 +17961,7 @@
         <v>0.58823529411764719</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>31</v>
       </c>
@@ -18021,7 +18020,7 @@
         <v>0.62352941176470589</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>32</v>
       </c>
@@ -18080,7 +18079,7 @@
         <v>0.51764705882352935</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -18139,7 +18138,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>34</v>
       </c>
@@ -18198,7 +18197,7 @@
         <v>0.58823529411764719</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>35</v>
       </c>
@@ -18257,7 +18256,7 @@
         <v>0.48235294117647071</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>36</v>
       </c>
@@ -18316,7 +18315,7 @@
         <v>0.55294117647058805</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>37</v>
       </c>
@@ -18375,7 +18374,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>38</v>
       </c>
@@ -18434,7 +18433,7 @@
         <v>0.48235294117647071</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>39</v>
       </c>
@@ -18493,7 +18492,7 @@
         <v>0.69411764705882351</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>40</v>
       </c>
@@ -18552,7 +18551,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>41</v>
       </c>
@@ -18611,7 +18610,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>42</v>
       </c>
@@ -18670,7 +18669,7 @@
         <v>0.55294117647058805</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>43</v>
       </c>
@@ -18729,7 +18728,7 @@
         <v>0.76470588235294135</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>44</v>
       </c>
@@ -18788,7 +18787,7 @@
         <v>0.65882352941176481</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>45</v>
       </c>
@@ -18847,7 +18846,7 @@
         <v>0.44705882352941173</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>46</v>
       </c>
@@ -18906,7 +18905,7 @@
         <v>0.69411764705882351</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>47</v>
       </c>
@@ -18965,7 +18964,7 @@
         <v>0.58823529411764719</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>48</v>
       </c>
@@ -19024,7 +19023,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>49</v>
       </c>
@@ -19083,7 +19082,7 @@
         <v>0.376470588235294</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>50</v>
       </c>
@@ -19142,7 +19141,7 @@
         <v>0.65882352941176481</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>51</v>
       </c>
@@ -19201,7 +19200,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>52</v>
       </c>
@@ -19260,7 +19259,7 @@
         <v>0.62352941176470589</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>53</v>
       </c>
@@ -19319,7 +19318,7 @@
         <v>0.69411764705882351</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>54</v>
       </c>
@@ -19378,7 +19377,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>55</v>
       </c>
@@ -19437,7 +19436,7 @@
         <v>0.51764705882352935</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>56</v>
       </c>
@@ -19496,7 +19495,7 @@
         <v>0.44705882352941173</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>57</v>
       </c>
@@ -19555,7 +19554,7 @@
         <v>0.62352941176470589</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>58</v>
       </c>
@@ -19614,7 +19613,7 @@
         <v>0.55294117647058805</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>59</v>
       </c>
@@ -19673,7 +19672,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>60</v>
       </c>
@@ -19732,7 +19731,7 @@
         <v>0.7294117647058822</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>61</v>
       </c>
@@ -19791,7 +19790,7 @@
         <v>0.41176470588235303</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>62</v>
       </c>
@@ -19850,7 +19849,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="14" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:19" ht="13.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>63</v>
       </c>
@@ -19921,19 +19920,19 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="4" width="20.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -19947,70 +19946,70 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="28" t="s">
         <v>28</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="28" t="s">
         <v>33</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="28" t="s">
         <v>34</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="28" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="28" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="10" t="s">

</xml_diff>